<commit_message>
updated with new define.
</commit_message>
<xml_diff>
--- a/adam/TDF_ADaM - Pilot 3 Team updated.xlsx
+++ b/adam/TDF_ADaM - Pilot 3 Team updated.xlsx
@@ -31,14 +31,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId15" roundtripDataSignature="AMtx7mjlIiopTC2j3ezfSm/6ZEXgAkaX8g=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId15" roundtripDataSignature="AMtx7mg/JFUxQOmTIubPDxhj1CHsCKEWpQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5230" uniqueCount="1288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5229" uniqueCount="1288">
   <si>
     <t>Attribute</t>
   </si>
@@ -3928,7 +3928,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -3979,15 +3978,21 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -9479,11 +9484,11 @@
       <c r="E28" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>83</v>
+      <c r="F28" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G28" s="5">
+        <v>13.0</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>27</v>
@@ -15320,7 +15325,7 @@
       <c r="C210" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="D210" s="4" t="s">
+      <c r="D210" s="6" t="s">
         <v>600</v>
       </c>
       <c r="E210" s="2" t="s">
@@ -16472,11 +16477,11 @@
       <c r="F2" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>83</v>
+      <c r="G2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>27</v>
@@ -16507,11 +16512,11 @@
       <c r="F3" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>83</v>
+      <c r="G3" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>27</v>
@@ -16542,11 +16547,11 @@
       <c r="F4" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>83</v>
+      <c r="G4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>27</v>
@@ -16577,11 +16582,11 @@
       <c r="F5" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>83</v>
+      <c r="G5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>27</v>
@@ -16612,11 +16617,11 @@
       <c r="F6" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>83</v>
+      <c r="G6" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>27</v>
@@ -16647,11 +16652,11 @@
       <c r="F7" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>83</v>
+      <c r="G7" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>27</v>
@@ -16682,11 +16687,11 @@
       <c r="F8" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>83</v>
+      <c r="G8" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>27</v>
@@ -16717,11 +16722,11 @@
       <c r="F9" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>83</v>
+      <c r="G9" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>27</v>
@@ -16752,11 +16757,11 @@
       <c r="F10" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>83</v>
+      <c r="G10" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>27</v>
@@ -16787,11 +16792,11 @@
       <c r="F11" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>83</v>
+      <c r="G11" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>27</v>
@@ -16822,11 +16827,11 @@
       <c r="F12" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>83</v>
+      <c r="G12" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>27</v>
@@ -16857,11 +16862,11 @@
       <c r="F13" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>83</v>
+      <c r="G13" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>27</v>
@@ -16892,11 +16897,11 @@
       <c r="F14" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>83</v>
+      <c r="G14" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>27</v>
@@ -16927,11 +16932,11 @@
       <c r="F15" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>83</v>
+      <c r="G15" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>27</v>
@@ -16962,11 +16967,11 @@
       <c r="F16" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>83</v>
+      <c r="G16" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>27</v>
@@ -26699,7 +26704,7 @@
       <c r="C2" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>964</v>
       </c>
     </row>
@@ -26713,7 +26718,7 @@
       <c r="C3" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>966</v>
       </c>
     </row>
@@ -26727,7 +26732,7 @@
       <c r="C4" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="7" t="s">
         <v>968</v>
       </c>
     </row>
@@ -26741,7 +26746,7 @@
       <c r="C5" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="7" t="s">
         <v>970</v>
       </c>
     </row>
@@ -26755,7 +26760,7 @@
       <c r="C6" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="7" t="s">
         <v>972</v>
       </c>
     </row>
@@ -26769,7 +26774,7 @@
       <c r="C7" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="7" t="s">
         <v>974</v>
       </c>
     </row>
@@ -26783,7 +26788,7 @@
       <c r="C8" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="7" t="s">
         <v>976</v>
       </c>
     </row>
@@ -26797,7 +26802,7 @@
       <c r="C9" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="7" t="s">
         <v>978</v>
       </c>
     </row>
@@ -26811,7 +26816,7 @@
       <c r="C10" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="7" t="s">
         <v>980</v>
       </c>
     </row>
@@ -26825,7 +26830,7 @@
       <c r="C11" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="7" t="s">
         <v>982</v>
       </c>
     </row>
@@ -26839,7 +26844,7 @@
       <c r="C12" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="7" t="s">
         <v>984</v>
       </c>
     </row>
@@ -26853,7 +26858,7 @@
       <c r="C13" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="7" t="s">
         <v>986</v>
       </c>
     </row>
@@ -26867,7 +26872,7 @@
       <c r="C14" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="7" t="s">
         <v>988</v>
       </c>
     </row>
@@ -26881,7 +26886,7 @@
       <c r="C15" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="7" t="s">
         <v>990</v>
       </c>
     </row>
@@ -26895,7 +26900,7 @@
       <c r="C16" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="7" t="s">
         <v>992</v>
       </c>
     </row>
@@ -26909,7 +26914,7 @@
       <c r="C17" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="7" t="s">
         <v>994</v>
       </c>
     </row>
@@ -26923,7 +26928,7 @@
       <c r="C18" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="7" t="s">
         <v>996</v>
       </c>
     </row>
@@ -26937,7 +26942,7 @@
       <c r="C19" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="7" t="s">
         <v>998</v>
       </c>
     </row>
@@ -26951,7 +26956,7 @@
       <c r="C20" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="7" t="s">
         <v>1000</v>
       </c>
     </row>
@@ -26965,7 +26970,7 @@
       <c r="C21" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="7" t="s">
         <v>1002</v>
       </c>
     </row>
@@ -26979,7 +26984,7 @@
       <c r="C22" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="7" t="s">
         <v>1004</v>
       </c>
     </row>
@@ -26993,7 +26998,7 @@
       <c r="C23" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="7" t="s">
         <v>1006</v>
       </c>
     </row>
@@ -27007,7 +27012,7 @@
       <c r="C24" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="7" t="s">
         <v>1008</v>
       </c>
     </row>
@@ -27021,7 +27026,7 @@
       <c r="C25" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="7" t="s">
         <v>1010</v>
       </c>
     </row>
@@ -27035,7 +27040,7 @@
       <c r="C26" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="7" t="s">
         <v>1012</v>
       </c>
     </row>
@@ -27049,7 +27054,7 @@
       <c r="C27" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="7" t="s">
         <v>1014</v>
       </c>
     </row>
@@ -27063,7 +27068,7 @@
       <c r="C28" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="7" t="s">
         <v>1016</v>
       </c>
     </row>
@@ -27077,7 +27082,7 @@
       <c r="C29" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="7" t="s">
         <v>1018</v>
       </c>
     </row>
@@ -27091,7 +27096,7 @@
       <c r="C30" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="7" t="s">
         <v>1020</v>
       </c>
     </row>
@@ -27105,7 +27110,7 @@
       <c r="C31" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="7" t="s">
         <v>1022</v>
       </c>
     </row>
@@ -27119,7 +27124,7 @@
       <c r="C32" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="7" t="s">
         <v>1024</v>
       </c>
     </row>
@@ -27133,7 +27138,7 @@
       <c r="C33" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="7" t="s">
         <v>1026</v>
       </c>
     </row>
@@ -27147,7 +27152,7 @@
       <c r="C34" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="7" t="s">
         <v>1028</v>
       </c>
     </row>
@@ -27161,7 +27166,7 @@
       <c r="C35" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="7" t="s">
         <v>1030</v>
       </c>
     </row>
@@ -27175,7 +27180,7 @@
       <c r="C36" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="7" t="s">
         <v>1032</v>
       </c>
     </row>
@@ -27189,7 +27194,7 @@
       <c r="C37" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="7" t="s">
         <v>1034</v>
       </c>
     </row>
@@ -27203,7 +27208,7 @@
       <c r="C38" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="7" t="s">
         <v>1036</v>
       </c>
     </row>
@@ -27217,7 +27222,7 @@
       <c r="C39" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="7" t="s">
         <v>1038</v>
       </c>
     </row>
@@ -27231,7 +27236,7 @@
       <c r="C40" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="7" t="s">
         <v>1040</v>
       </c>
     </row>
@@ -27245,7 +27250,7 @@
       <c r="C41" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="7" t="s">
         <v>1042</v>
       </c>
     </row>
@@ -27259,7 +27264,7 @@
       <c r="C42" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="7" t="s">
         <v>500</v>
       </c>
     </row>
@@ -27273,7 +27278,7 @@
       <c r="C43" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="7" t="s">
         <v>107</v>
       </c>
     </row>
@@ -27287,7 +27292,7 @@
       <c r="C44" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="7" t="s">
         <v>110</v>
       </c>
     </row>
@@ -27301,7 +27306,7 @@
       <c r="C45" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="7" t="s">
         <v>1047</v>
       </c>
     </row>
@@ -27315,7 +27320,7 @@
       <c r="C46" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="7" t="s">
         <v>1049</v>
       </c>
     </row>
@@ -27329,7 +27334,7 @@
       <c r="C47" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="7" t="s">
         <v>1051</v>
       </c>
     </row>
@@ -27343,7 +27348,7 @@
       <c r="C48" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="7" t="s">
         <v>1053</v>
       </c>
     </row>
@@ -27357,7 +27362,7 @@
       <c r="C49" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="7" t="s">
         <v>1055</v>
       </c>
     </row>
@@ -27371,7 +27376,7 @@
       <c r="C50" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="7" t="s">
         <v>1057</v>
       </c>
     </row>
@@ -27385,7 +27390,7 @@
       <c r="C51" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="7" t="s">
         <v>1059</v>
       </c>
     </row>
@@ -27399,7 +27404,7 @@
       <c r="C52" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="7" t="s">
         <v>1061</v>
       </c>
     </row>
@@ -27413,7 +27418,7 @@
       <c r="C53" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="7" t="s">
         <v>1063</v>
       </c>
     </row>
@@ -27427,7 +27432,7 @@
       <c r="C54" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="7" t="s">
         <v>1065</v>
       </c>
     </row>
@@ -27441,7 +27446,7 @@
       <c r="C55" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="7" t="s">
         <v>1067</v>
       </c>
     </row>
@@ -27455,7 +27460,7 @@
       <c r="C56" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" s="7" t="s">
         <v>504</v>
       </c>
     </row>
@@ -27469,7 +27474,7 @@
       <c r="C57" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="7" t="s">
         <v>118</v>
       </c>
     </row>
@@ -27483,7 +27488,7 @@
       <c r="C58" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="7" t="s">
         <v>509</v>
       </c>
     </row>
@@ -27497,7 +27502,7 @@
       <c r="C59" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="7" t="s">
         <v>505</v>
       </c>
     </row>
@@ -27511,7 +27516,7 @@
       <c r="C60" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="7" t="s">
         <v>477</v>
       </c>
     </row>
@@ -27525,7 +27530,7 @@
       <c r="C61" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="7" t="s">
         <v>474</v>
       </c>
     </row>
@@ -27539,7 +27544,7 @@
       <c r="C62" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="7" t="s">
         <v>487</v>
       </c>
     </row>
@@ -27553,7 +27558,7 @@
       <c r="C63" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="7" t="s">
         <v>490</v>
       </c>
     </row>
@@ -27567,7 +27572,7 @@
       <c r="C64" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="7" t="s">
         <v>89</v>
       </c>
     </row>
@@ -27581,7 +27586,7 @@
       <c r="C65" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="7" t="s">
         <v>1078</v>
       </c>
     </row>
@@ -27595,7 +27600,7 @@
       <c r="C66" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" s="7" t="s">
         <v>85</v>
       </c>
     </row>
@@ -27609,7 +27614,7 @@
       <c r="C67" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" s="7" t="s">
         <v>1081</v>
       </c>
     </row>
@@ -27623,7 +27628,7 @@
       <c r="C68" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D68" s="7" t="s">
         <v>1083</v>
       </c>
     </row>
@@ -27637,7 +27642,7 @@
       <c r="C69" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" s="7" t="s">
         <v>1085</v>
       </c>
     </row>
@@ -27651,7 +27656,7 @@
       <c r="C70" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" s="7" t="s">
         <v>1087</v>
       </c>
     </row>
@@ -27665,7 +27670,7 @@
       <c r="C71" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D71" s="7" t="s">
         <v>1089</v>
       </c>
     </row>
@@ -27679,7 +27684,7 @@
       <c r="C72" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="7" t="s">
         <v>1091</v>
       </c>
     </row>
@@ -27693,7 +27698,7 @@
       <c r="C73" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D73" s="7" t="s">
         <v>500</v>
       </c>
     </row>
@@ -27707,7 +27712,7 @@
       <c r="C74" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="7" t="s">
         <v>107</v>
       </c>
     </row>
@@ -27721,7 +27726,7 @@
       <c r="C75" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="7" t="s">
         <v>110</v>
       </c>
     </row>
@@ -27735,7 +27740,7 @@
       <c r="C76" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="7" t="s">
         <v>1096</v>
       </c>
     </row>
@@ -27749,7 +27754,7 @@
       <c r="C77" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="7" t="s">
         <v>1081</v>
       </c>
     </row>
@@ -27763,7 +27768,7 @@
       <c r="C78" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="7" t="s">
         <v>1081</v>
       </c>
     </row>
@@ -27777,7 +27782,7 @@
       <c r="C79" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D79" s="7" t="s">
         <v>1081</v>
       </c>
     </row>
@@ -27791,7 +27796,7 @@
       <c r="C80" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="D80" s="7" t="s">
         <v>138</v>
       </c>
     </row>
@@ -27805,7 +27810,7 @@
       <c r="C81" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" s="7" t="s">
         <v>976</v>
       </c>
     </row>
@@ -27819,7 +27824,7 @@
       <c r="C82" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D82" s="7" t="s">
         <v>1081</v>
       </c>
     </row>
@@ -27833,7 +27838,7 @@
       <c r="C83" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D83" s="7" t="s">
         <v>1081</v>
       </c>
     </row>
@@ -27847,7 +27852,7 @@
       <c r="C84" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="7" t="s">
         <v>1105</v>
       </c>
     </row>
@@ -27861,7 +27866,7 @@
       <c r="C85" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D85" s="7" t="s">
         <v>1107</v>
       </c>
     </row>
@@ -27875,7 +27880,7 @@
       <c r="C86" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="D86" s="7" t="s">
         <v>1081</v>
       </c>
     </row>
@@ -27889,7 +27894,7 @@
       <c r="C87" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D87" s="7" t="s">
         <v>135</v>
       </c>
     </row>
@@ -27903,7 +27908,7 @@
       <c r="C88" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="7" t="s">
         <v>519</v>
       </c>
     </row>
@@ -27917,7 +27922,7 @@
       <c r="C89" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="D89" s="7" t="s">
         <v>1112</v>
       </c>
     </row>
@@ -27931,7 +27936,7 @@
       <c r="C90" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="D90" s="7" t="s">
         <v>1114</v>
       </c>
     </row>
@@ -27945,7 +27950,7 @@
       <c r="C91" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="D91" s="7" t="s">
         <v>1116</v>
       </c>
     </row>
@@ -27959,7 +27964,7 @@
       <c r="C92" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="D92" s="7" t="s">
         <v>1118</v>
       </c>
     </row>
@@ -27973,7 +27978,7 @@
       <c r="C93" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="D93" s="7" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -27987,7 +27992,7 @@
       <c r="C94" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D94" s="7" t="s">
         <v>1122</v>
       </c>
     </row>
@@ -28001,7 +28006,7 @@
       <c r="C95" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D95" s="7" t="s">
         <v>1124</v>
       </c>
     </row>
@@ -28015,7 +28020,7 @@
       <c r="C96" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D96" s="7" t="s">
         <v>1126</v>
       </c>
     </row>
@@ -28029,7 +28034,7 @@
       <c r="C97" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="D97" s="7" t="s">
         <v>1128</v>
       </c>
     </row>
@@ -28043,7 +28048,7 @@
       <c r="C98" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="D98" s="7" t="s">
         <v>504</v>
       </c>
     </row>
@@ -28057,7 +28062,7 @@
       <c r="C99" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="D99" s="7" t="s">
         <v>118</v>
       </c>
     </row>
@@ -28071,7 +28076,7 @@
       <c r="C100" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D100" s="7" t="s">
         <v>509</v>
       </c>
     </row>
@@ -28085,7 +28090,7 @@
       <c r="C101" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="D101" s="7" t="s">
         <v>505</v>
       </c>
     </row>
@@ -28099,7 +28104,7 @@
       <c r="C102" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D102" s="7" t="s">
         <v>474</v>
       </c>
     </row>
@@ -28113,7 +28118,7 @@
       <c r="C103" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="D103" s="7" t="s">
         <v>476</v>
       </c>
     </row>
@@ -28127,7 +28132,7 @@
       <c r="C104" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D104" s="5" t="s">
+      <c r="D104" s="7" t="s">
         <v>487</v>
       </c>
     </row>
@@ -28141,7 +28146,7 @@
       <c r="C105" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D105" s="5" t="s">
+      <c r="D105" s="7" t="s">
         <v>490</v>
       </c>
     </row>
@@ -28155,7 +28160,7 @@
       <c r="C106" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D106" s="5" t="s">
+      <c r="D106" s="7" t="s">
         <v>89</v>
       </c>
     </row>
@@ -28169,7 +28174,7 @@
       <c r="C107" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D107" s="5" t="s">
+      <c r="D107" s="7" t="s">
         <v>482</v>
       </c>
     </row>
@@ -28183,7 +28188,7 @@
       <c r="C108" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D108" s="5" t="s">
+      <c r="D108" s="7" t="s">
         <v>99</v>
       </c>
     </row>
@@ -28197,7 +28202,7 @@
       <c r="C109" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D109" s="5" t="s">
+      <c r="D109" s="7" t="s">
         <v>85</v>
       </c>
     </row>
@@ -28211,7 +28216,7 @@
       <c r="C110" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D110" s="5" t="s">
+      <c r="D110" s="7" t="s">
         <v>103</v>
       </c>
     </row>
@@ -28225,7 +28230,7 @@
       <c r="C111" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D111" s="5" t="s">
+      <c r="D111" s="7" t="s">
         <v>1143</v>
       </c>
     </row>
@@ -28239,7 +28244,7 @@
       <c r="C112" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D112" s="5" t="s">
+      <c r="D112" s="7" t="s">
         <v>1145</v>
       </c>
     </row>
@@ -28253,7 +28258,7 @@
       <c r="C113" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D113" s="5" t="s">
+      <c r="D113" s="7" t="s">
         <v>1147</v>
       </c>
     </row>
@@ -28267,7 +28272,7 @@
       <c r="C114" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D114" s="5" t="s">
+      <c r="D114" s="7" t="s">
         <v>95</v>
       </c>
     </row>
@@ -28281,7 +28286,7 @@
       <c r="C115" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D115" s="5" t="s">
+      <c r="D115" s="7" t="s">
         <v>1150</v>
       </c>
     </row>
@@ -28295,7 +28300,7 @@
       <c r="C116" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D116" s="5" t="s">
+      <c r="D116" s="7" t="s">
         <v>1152</v>
       </c>
     </row>
@@ -28309,7 +28314,7 @@
       <c r="C117" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D117" s="5" t="s">
+      <c r="D117" s="7" t="s">
         <v>1154</v>
       </c>
     </row>
@@ -28323,7 +28328,7 @@
       <c r="C118" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D118" s="5" t="s">
+      <c r="D118" s="7" t="s">
         <v>1156</v>
       </c>
     </row>
@@ -28337,7 +28342,7 @@
       <c r="C119" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D119" s="5" t="s">
+      <c r="D119" s="7" t="s">
         <v>1158</v>
       </c>
     </row>
@@ -28351,7 +28356,7 @@
       <c r="C120" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D120" s="5" t="s">
+      <c r="D120" s="7" t="s">
         <v>1160</v>
       </c>
     </row>
@@ -28365,7 +28370,7 @@
       <c r="C121" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D121" s="5" t="s">
+      <c r="D121" s="7" t="s">
         <v>1162</v>
       </c>
     </row>
@@ -28379,7 +28384,7 @@
       <c r="C122" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D122" s="5" t="s">
+      <c r="D122" s="7" t="s">
         <v>1164</v>
       </c>
     </row>
@@ -28393,7 +28398,7 @@
       <c r="C123" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D123" s="5" t="s">
+      <c r="D123" s="7" t="s">
         <v>1166</v>
       </c>
     </row>
@@ -28407,7 +28412,7 @@
       <c r="C124" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D124" s="5" t="s">
+      <c r="D124" s="7" t="s">
         <v>1168</v>
       </c>
     </row>
@@ -28421,7 +28426,7 @@
       <c r="C125" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D125" s="5" t="s">
+      <c r="D125" s="7" t="s">
         <v>1170</v>
       </c>
     </row>
@@ -28435,7 +28440,7 @@
       <c r="C126" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D126" s="5" t="s">
+      <c r="D126" s="7" t="s">
         <v>1172</v>
       </c>
     </row>
@@ -28449,7 +28454,7 @@
       <c r="C127" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D127" s="5" t="s">
+      <c r="D127" s="7" t="s">
         <v>1174</v>
       </c>
     </row>
@@ -28463,7 +28468,7 @@
       <c r="C128" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D128" s="5" t="s">
+      <c r="D128" s="7" t="s">
         <v>1176</v>
       </c>
     </row>
@@ -28477,7 +28482,7 @@
       <c r="C129" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D129" s="5" t="s">
+      <c r="D129" s="7" t="s">
         <v>1178</v>
       </c>
     </row>
@@ -28491,7 +28496,7 @@
       <c r="C130" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D130" s="5" t="s">
+      <c r="D130" s="7" t="s">
         <v>1180</v>
       </c>
     </row>
@@ -28505,7 +28510,7 @@
       <c r="C131" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D131" s="5" t="s">
+      <c r="D131" s="7" t="s">
         <v>1182</v>
       </c>
     </row>
@@ -28519,7 +28524,7 @@
       <c r="C132" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D132" s="5" t="s">
+      <c r="D132" s="7" t="s">
         <v>1184</v>
       </c>
     </row>
@@ -28533,7 +28538,7 @@
       <c r="C133" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D133" s="5" t="s">
+      <c r="D133" s="7" t="s">
         <v>1186</v>
       </c>
     </row>
@@ -28547,7 +28552,7 @@
       <c r="C134" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D134" s="5" t="s">
+      <c r="D134" s="7" t="s">
         <v>1188</v>
       </c>
     </row>
@@ -28561,7 +28566,7 @@
       <c r="C135" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D135" s="5" t="s">
+      <c r="D135" s="7" t="s">
         <v>1190</v>
       </c>
     </row>
@@ -28575,7 +28580,7 @@
       <c r="C136" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D136" s="5" t="s">
+      <c r="D136" s="7" t="s">
         <v>1192</v>
       </c>
     </row>
@@ -28589,7 +28594,7 @@
       <c r="C137" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D137" s="5" t="s">
+      <c r="D137" s="7" t="s">
         <v>114</v>
       </c>
     </row>
@@ -28603,7 +28608,7 @@
       <c r="C138" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D138" s="5" t="s">
+      <c r="D138" s="7" t="s">
         <v>1195</v>
       </c>
     </row>
@@ -28617,7 +28622,7 @@
       <c r="C139" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D139" s="5" t="s">
+      <c r="D139" s="7" t="s">
         <v>1197</v>
       </c>
     </row>
@@ -28631,7 +28636,7 @@
       <c r="C140" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D140" s="5" t="s">
+      <c r="D140" s="7" t="s">
         <v>1199</v>
       </c>
     </row>
@@ -28645,7 +28650,7 @@
       <c r="C141" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D141" s="5" t="s">
+      <c r="D141" s="7" t="s">
         <v>1201</v>
       </c>
     </row>
@@ -28659,7 +28664,7 @@
       <c r="C142" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D142" s="5" t="s">
+      <c r="D142" s="7" t="s">
         <v>1203</v>
       </c>
     </row>
@@ -28673,7 +28678,7 @@
       <c r="C143" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D143" s="5" t="s">
+      <c r="D143" s="7" t="s">
         <v>122</v>
       </c>
     </row>
@@ -28687,7 +28692,7 @@
       <c r="C144" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D144" s="5" t="s">
+      <c r="D144" s="7" t="s">
         <v>1206</v>
       </c>
     </row>
@@ -28701,7 +28706,7 @@
       <c r="C145" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D145" s="5" t="s">
+      <c r="D145" s="7" t="s">
         <v>71</v>
       </c>
     </row>
@@ -28715,7 +28720,7 @@
       <c r="C146" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D146" s="5" t="s">
+      <c r="D146" s="7" t="s">
         <v>66</v>
       </c>
     </row>
@@ -28729,7 +28734,7 @@
       <c r="C147" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D147" s="5" t="s">
+      <c r="D147" s="7" t="s">
         <v>1210</v>
       </c>
     </row>
@@ -28743,7 +28748,7 @@
       <c r="C148" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D148" s="5" t="s">
+      <c r="D148" s="7" t="s">
         <v>1212</v>
       </c>
     </row>
@@ -28757,7 +28762,7 @@
       <c r="C149" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D149" s="5" t="s">
+      <c r="D149" s="7" t="s">
         <v>1214</v>
       </c>
     </row>
@@ -28771,7 +28776,7 @@
       <c r="C150" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D150" s="5" t="s">
+      <c r="D150" s="7" t="s">
         <v>95</v>
       </c>
     </row>
@@ -28785,7 +28790,7 @@
       <c r="C151" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D151" s="5" t="s">
+      <c r="D151" s="7" t="s">
         <v>1217</v>
       </c>
     </row>
@@ -28799,7 +28804,7 @@
       <c r="C152" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D152" s="5" t="s">
+      <c r="D152" s="7" t="s">
         <v>1219</v>
       </c>
     </row>
@@ -28813,7 +28818,7 @@
       <c r="C153" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D153" s="5" t="s">
+      <c r="D153" s="7" t="s">
         <v>1221</v>
       </c>
     </row>
@@ -28827,7 +28832,7 @@
       <c r="C154" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D154" s="5" t="s">
+      <c r="D154" s="7" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -28841,7 +28846,7 @@
       <c r="C155" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D155" s="5" t="s">
+      <c r="D155" s="7" t="s">
         <v>1225</v>
       </c>
     </row>
@@ -28855,7 +28860,7 @@
       <c r="C156" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D156" s="5" t="s">
+      <c r="D156" s="7" t="s">
         <v>1227</v>
       </c>
     </row>
@@ -28869,7 +28874,7 @@
       <c r="C157" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D157" s="5" t="s">
+      <c r="D157" s="7" t="s">
         <v>1229</v>
       </c>
     </row>
@@ -28883,7 +28888,7 @@
       <c r="C158" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D158" s="5" t="s">
+      <c r="D158" s="7" t="s">
         <v>1231</v>
       </c>
     </row>
@@ -28897,7 +28902,7 @@
       <c r="C159" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D159" s="5" t="s">
+      <c r="D159" s="7" t="s">
         <v>500</v>
       </c>
     </row>
@@ -28911,7 +28916,7 @@
       <c r="C160" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D160" s="5" t="s">
+      <c r="D160" s="7" t="s">
         <v>107</v>
       </c>
     </row>
@@ -28925,7 +28930,7 @@
       <c r="C161" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D161" s="5" t="s">
+      <c r="D161" s="7" t="s">
         <v>110</v>
       </c>
     </row>
@@ -28939,7 +28944,7 @@
       <c r="C162" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D162" s="5" t="s">
+      <c r="D162" s="7" t="s">
         <v>1236</v>
       </c>
     </row>
@@ -28953,7 +28958,7 @@
       <c r="C163" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D163" s="5" t="s">
+      <c r="D163" s="7" t="s">
         <v>1238</v>
       </c>
     </row>
@@ -28967,7 +28972,7 @@
       <c r="C164" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D164" s="5" t="s">
+      <c r="D164" s="7" t="s">
         <v>1240</v>
       </c>
     </row>
@@ -28981,7 +28986,7 @@
       <c r="C165" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D165" s="5" t="s">
+      <c r="D165" s="7" t="s">
         <v>1242</v>
       </c>
     </row>
@@ -28995,7 +29000,7 @@
       <c r="C166" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D166" s="5" t="s">
+      <c r="D166" s="7" t="s">
         <v>1244</v>
       </c>
     </row>
@@ -29009,7 +29014,7 @@
       <c r="C167" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D167" s="5" t="s">
+      <c r="D167" s="7" t="s">
         <v>504</v>
       </c>
     </row>
@@ -29023,7 +29028,7 @@
       <c r="C168" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D168" s="5" t="s">
+      <c r="D168" s="7" t="s">
         <v>118</v>
       </c>
     </row>
@@ -29037,7 +29042,7 @@
       <c r="C169" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D169" s="5" t="s">
+      <c r="D169" s="7" t="s">
         <v>509</v>
       </c>
     </row>
@@ -29051,7 +29056,7 @@
       <c r="C170" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D170" s="5" t="s">
+      <c r="D170" s="7" t="s">
         <v>505</v>
       </c>
     </row>
@@ -29065,7 +29070,7 @@
       <c r="C171" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D171" s="5" t="s">
+      <c r="D171" s="7" t="s">
         <v>477</v>
       </c>
     </row>
@@ -29079,7 +29084,7 @@
       <c r="C172" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D172" s="5" t="s">
+      <c r="D172" s="7" t="s">
         <v>1251</v>
       </c>
     </row>
@@ -29093,7 +29098,7 @@
       <c r="C173" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D173" s="5" t="s">
+      <c r="D173" s="7" t="s">
         <v>1253</v>
       </c>
     </row>
@@ -29107,7 +29112,7 @@
       <c r="C174" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D174" s="5" t="s">
+      <c r="D174" s="7" t="s">
         <v>1255</v>
       </c>
     </row>
@@ -29121,7 +29126,7 @@
       <c r="C175" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D175" s="5" t="s">
+      <c r="D175" s="7" t="s">
         <v>554</v>
       </c>
     </row>
@@ -29135,7 +29140,7 @@
       <c r="C176" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D176" s="5" t="s">
+      <c r="D176" s="7" t="s">
         <v>474</v>
       </c>
     </row>
@@ -29149,7 +29154,7 @@
       <c r="C177" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D177" s="5" t="s">
+      <c r="D177" s="7" t="s">
         <v>487</v>
       </c>
     </row>
@@ -29163,7 +29168,7 @@
       <c r="C178" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D178" s="5" t="s">
+      <c r="D178" s="7" t="s">
         <v>490</v>
       </c>
     </row>
@@ -29177,7 +29182,7 @@
       <c r="C179" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D179" s="5" t="s">
+      <c r="D179" s="7" t="s">
         <v>493</v>
       </c>
     </row>
@@ -29191,7 +29196,7 @@
       <c r="C180" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D180" s="5" t="s">
+      <c r="D180" s="7" t="s">
         <v>89</v>
       </c>
     </row>
@@ -29205,7 +29210,7 @@
       <c r="C181" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D181" s="5" t="s">
+      <c r="D181" s="7" t="s">
         <v>482</v>
       </c>
     </row>
@@ -29219,7 +29224,7 @@
       <c r="C182" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="D182" s="5" t="s">
+      <c r="D182" s="7" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>